<commit_message>
added multiple category option
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E71C0D6-01AE-45B4-BFE8-7C1C249AB71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF39399F-8BAF-4C36-A2C7-40DB33B05329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="2265" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Armory</t>
-  </si>
-  <si>
     <t>Building set</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>f4.jpg</t>
+  </si>
+  <si>
+    <t>Armory, Cosplay</t>
   </si>
 </sst>
 </file>
@@ -141,8 +141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,113 +463,113 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
         <v>8500</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
         <v>4200</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
         <v>1200</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
         <v>2000</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
         <v>2200</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
         <v>1700</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed create order to home in preorder
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF39399F-8BAF-4C36-A2C7-40DB33B05329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6709EE5-684A-48D4-BAD7-0D77339EE98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="2265" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
stock and pre-order updated
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6709EE5-684A-48D4-BAD7-0D77339EE98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFF6DCC-1255-47EF-B33A-5756CB0749CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="2265" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Product</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Gunpla</t>
   </si>
   <si>
-    <t>placeholder.jpg</t>
-  </si>
-  <si>
     <t>slide3.jpg</t>
   </si>
   <si>
@@ -100,6 +97,75 @@
   </si>
   <si>
     <t>Armory, Cosplay</t>
+  </si>
+  <si>
+    <t>Thor 1/12 Plastic Model Kit FondJoy</t>
+  </si>
+  <si>
+    <t>Spiderman 1/12 Plastic Model Kit FondJoy</t>
+  </si>
+  <si>
+    <t>Thanos 1/12 Plastic Model Kit FondJoy</t>
+  </si>
+  <si>
+    <t>Hulk 1/12 Plastic Model Kit FondJoy</t>
+  </si>
+  <si>
+    <t>Captain America 1/12 Plastic Model Kit FondJoy</t>
+  </si>
+  <si>
+    <t>thor fj.jpg</t>
+  </si>
+  <si>
+    <t>spiderman fj.jpg</t>
+  </si>
+  <si>
+    <t>thanos fj.jpg</t>
+  </si>
+  <si>
+    <t>cap fj.jpg</t>
+  </si>
+  <si>
+    <t>hulk fj.jpg</t>
+  </si>
+  <si>
+    <t>ironman gantry.jpg</t>
+  </si>
+  <si>
+    <t>Ironman Gantry 1/10 scale</t>
+  </si>
+  <si>
+    <t>new superman set.jpg</t>
+  </si>
+  <si>
+    <t>thunderbolts.jpg</t>
+  </si>
+  <si>
+    <t>thor love.jpg</t>
+  </si>
+  <si>
+    <t>small hog.jpg</t>
+  </si>
+  <si>
+    <t>Hogwarts Castle (Medium)</t>
+  </si>
+  <si>
+    <t>Hogwarts Castle (Large)</t>
+  </si>
+  <si>
+    <t>med hog.jpg</t>
+  </si>
+  <si>
+    <t>large hog.jpg</t>
+  </si>
+  <si>
+    <t>New Superman Movie Set (6 minifigure)</t>
+  </si>
+  <si>
+    <t>Thor - Love &amp; Thunder Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Thunderbolts Set (8 minifigure)</t>
   </si>
 </sst>
 </file>
@@ -460,18 +526,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B157F8F3-2502-4E5D-9075-AC3F10DBE2D5}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -490,21 +556,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>8500</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>4200</v>
@@ -513,26 +579,26 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>1200</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>2000</v>
@@ -541,12 +607,12 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>2200</v>
@@ -555,12 +621,12 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>1700</v>
@@ -569,7 +635,161 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1700</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1700</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1700</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1700</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1700</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="1">
+        <v>10500</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4500</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
image update in pre order
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFF6DCC-1255-47EF-B33A-5756CB0749CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B666DD70-0C24-4808-A4AA-72A8461EDDD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="2265" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>slide5.jpg</t>
   </si>
   <si>
-    <t>fj ironman.jpg</t>
-  </si>
-  <si>
     <t>hg freedom.jpg</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>Thunderbolts Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>ironman fj.jpg</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +562,7 @@
         <v>8500</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -593,7 +593,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -621,7 +621,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,12 +635,12 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
         <v>1700</v>
@@ -649,12 +649,12 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>1700</v>
@@ -663,12 +663,12 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1">
         <v>1700</v>
@@ -677,12 +677,12 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1">
         <v>1700</v>
@@ -691,12 +691,12 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>1700</v>
@@ -705,12 +705,12 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>10500</v>
@@ -719,12 +719,12 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1">
         <v>1600</v>
@@ -733,12 +733,12 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1">
         <v>1200</v>
@@ -747,12 +747,12 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1">
         <v>1600</v>
@@ -761,12 +761,12 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1">
         <v>3000</v>
@@ -775,12 +775,12 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1">
         <v>4500</v>
@@ -789,7 +789,7 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preorder update katana & cosplay
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2777163F-59CC-44BD-BCB5-7AD8EEEA9F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF991C73-C307-4560-B932-F0E402CF7FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="2265" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
+    <workbookView xWindow="4095" yWindow="735" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="161">
   <si>
     <t>Product</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Minifigure set</t>
   </si>
   <si>
-    <t>Ghost of Tsushima Katana</t>
-  </si>
-  <si>
     <t>Spiderman Mask</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>f4.jpg</t>
   </si>
   <si>
-    <t>Armory, Cosplay</t>
-  </si>
-  <si>
     <t>Thor 1/12 Plastic Model Kit FondJoy</t>
   </si>
   <si>
@@ -172,6 +166,357 @@
   </si>
   <si>
     <t>ironman gantry mark6.jpg</t>
+  </si>
+  <si>
+    <t>Armory</t>
+  </si>
+  <si>
+    <t>ame katana.jpg</t>
+  </si>
+  <si>
+    <t>Kikoku (Law's Katana) [Wooden]</t>
+  </si>
+  <si>
+    <t>Kitetsu II Katana [Wooden]</t>
+  </si>
+  <si>
+    <t>Shank's Sword [Wooden]</t>
+  </si>
+  <si>
+    <t>Roger's Sword [Wooden]</t>
+  </si>
+  <si>
+    <t>Enma (Black) Katana [Wooden]</t>
+  </si>
+  <si>
+    <t>Ame No Habikiri Katana [Wooden]</t>
+  </si>
+  <si>
+    <t>Enma (Purple) Katana [Wooden]</t>
+  </si>
+  <si>
+    <t>Shusui Katana [Wooden]</t>
+  </si>
+  <si>
+    <t>Wado Ichimonji Katana [Wooden]</t>
+  </si>
+  <si>
+    <t>Kitetsu III Katana [Wooden]</t>
+  </si>
+  <si>
+    <t>enma black katana.jpg</t>
+  </si>
+  <si>
+    <t>enma katana.jpg</t>
+  </si>
+  <si>
+    <t>shusui katana.jpg</t>
+  </si>
+  <si>
+    <t>wado katana.jpg</t>
+  </si>
+  <si>
+    <t>kitetsu katana.jpg</t>
+  </si>
+  <si>
+    <t>kitetsu 2 katana.jpg</t>
+  </si>
+  <si>
+    <t>shanks sword.jpg</t>
+  </si>
+  <si>
+    <t>roger sword.jpg</t>
+  </si>
+  <si>
+    <t>kikoku.jpg</t>
+  </si>
+  <si>
+    <t>Giyu's Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Giyu's Nichirin v2 [Wooden]</t>
+  </si>
+  <si>
+    <t>Rengoku Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Tanjiro's Old Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Tanjiro's New Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Sanemi's Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Kocho's Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Mitsuri's Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Muichiro's Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Inosuke Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Zenitsu's Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Kokushibo's Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Yorichi's Nichirin [Wooden]</t>
+  </si>
+  <si>
+    <t>Zoro' Katana Set [Wooden]</t>
+  </si>
+  <si>
+    <t>giyu katana.jpg</t>
+  </si>
+  <si>
+    <t>sanemi katana.jpg</t>
+  </si>
+  <si>
+    <t>kocho katana.jpg</t>
+  </si>
+  <si>
+    <t>mitsuri katana.jpg</t>
+  </si>
+  <si>
+    <t>muichiro katana.jpg</t>
+  </si>
+  <si>
+    <t>zenitsu katana.jpg</t>
+  </si>
+  <si>
+    <t>yorichi katana.jpg</t>
+  </si>
+  <si>
+    <t>giyu golden katana.jpg</t>
+  </si>
+  <si>
+    <t>rengoku katana.jpg</t>
+  </si>
+  <si>
+    <t>tanjiro old katana.jpg</t>
+  </si>
+  <si>
+    <t>tanjiro new katana.jpg</t>
+  </si>
+  <si>
+    <t>inosuke katana.jpg</t>
+  </si>
+  <si>
+    <t>kokushibo.jpg</t>
+  </si>
+  <si>
+    <t>zoro set katana.jpg</t>
+  </si>
+  <si>
+    <t>Venom Fang Dagger [Wooden]</t>
+  </si>
+  <si>
+    <t>Knight Killer Dagger [Wooden]</t>
+  </si>
+  <si>
+    <t>venom fang.jpg</t>
+  </si>
+  <si>
+    <t>knight killer.jpg</t>
+  </si>
+  <si>
+    <t>Ghost of Tsushima Katana [Metal]</t>
+  </si>
+  <si>
+    <t>Akatsuki Cloak</t>
+  </si>
+  <si>
+    <t>Attack on Titan Scout Cloak</t>
+  </si>
+  <si>
+    <t>akatsuki cosplay.jpg</t>
+  </si>
+  <si>
+    <t>aot cosplay.jpg</t>
+  </si>
+  <si>
+    <t>Batman Mask (Batman Begins)</t>
+  </si>
+  <si>
+    <t>Geto Cosplay Set</t>
+  </si>
+  <si>
+    <t>Giyu Cosplay Set</t>
+  </si>
+  <si>
+    <t>Itachi Cosplay Set</t>
+  </si>
+  <si>
+    <t>Obito Mask (Akatsuki)</t>
+  </si>
+  <si>
+    <t>Obito Mask (War)</t>
+  </si>
+  <si>
+    <t>Miles Morales Mask</t>
+  </si>
+  <si>
+    <t>miles mask.jpg</t>
+  </si>
+  <si>
+    <t>batman mask.jpg</t>
+  </si>
+  <si>
+    <t>obito mask.jpg</t>
+  </si>
+  <si>
+    <t>Zoro Cosplay (Classic)</t>
+  </si>
+  <si>
+    <t>Zoro Cosplay (Wano)</t>
+  </si>
+  <si>
+    <t>Zoro Cosplay (Onigashima)</t>
+  </si>
+  <si>
+    <t>Minato Cosplay Set</t>
+  </si>
+  <si>
+    <t>Luffy Cosplay (Onigashima)</t>
+  </si>
+  <si>
+    <t>Law Cosplay (Wano)</t>
+  </si>
+  <si>
+    <t>Kocho Cosplay Set</t>
+  </si>
+  <si>
+    <t>Nezuko Cosplay Set</t>
+  </si>
+  <si>
+    <t>Obanai Cosplay Set</t>
+  </si>
+  <si>
+    <t>Rengoku Cosplay Set</t>
+  </si>
+  <si>
+    <t>Tanjiro Cosplay Set</t>
+  </si>
+  <si>
+    <t>Zenitsu Cosplay Set</t>
+  </si>
+  <si>
+    <t>Gryffindor House Set</t>
+  </si>
+  <si>
+    <t>Ravenclaw Muffler [Large]</t>
+  </si>
+  <si>
+    <t>Hufflepuff Muffler [Large]</t>
+  </si>
+  <si>
+    <t>geto cosplay.jpg</t>
+  </si>
+  <si>
+    <t>itachi cosplay.jpg</t>
+  </si>
+  <si>
+    <t>giyu cosplay.jpg</t>
+  </si>
+  <si>
+    <t>kocho cosplay.jpg</t>
+  </si>
+  <si>
+    <t>tanjiro cosplay.jpg</t>
+  </si>
+  <si>
+    <t>nezuko cosplay.jpg</t>
+  </si>
+  <si>
+    <t>obanai cosplay.jpg</t>
+  </si>
+  <si>
+    <t>rengoku cosplay.jpg</t>
+  </si>
+  <si>
+    <t>zenitsu cosplay.jpg</t>
+  </si>
+  <si>
+    <t>minato cosplay set.jpg</t>
+  </si>
+  <si>
+    <t>obito mask war.jpg</t>
+  </si>
+  <si>
+    <t>zoro cosplay classic.jpg</t>
+  </si>
+  <si>
+    <t>zoro cosplay oni.jpg</t>
+  </si>
+  <si>
+    <t>zoro cosplay wano.jpg</t>
+  </si>
+  <si>
+    <t>luffy cosplay oni.jpg</t>
+  </si>
+  <si>
+    <t>law cosplay wano.jpg</t>
+  </si>
+  <si>
+    <t>law cosplay punk.jpg</t>
+  </si>
+  <si>
+    <t>gryf set.jpg</t>
+  </si>
+  <si>
+    <t>huff l muff.jpg</t>
+  </si>
+  <si>
+    <t>raven l muff.jpg</t>
+  </si>
+  <si>
+    <t>mitsuri cosplay.jpg</t>
+  </si>
+  <si>
+    <t>Mitsuri Cosplay Set</t>
+  </si>
+  <si>
+    <t>Gojo Cosplay Set</t>
+  </si>
+  <si>
+    <t>Itadori Cosplay Set</t>
+  </si>
+  <si>
+    <t>gojo cosplay.jpg</t>
+  </si>
+  <si>
+    <t>itadori cosplay.jpg</t>
+  </si>
+  <si>
+    <t>TBA</t>
+  </si>
+  <si>
+    <t>Law Cosplay (Punk Hazard)</t>
+  </si>
+  <si>
+    <t>Ichigo's Tensa Zangetsu Fullbring Bankai</t>
+  </si>
+  <si>
+    <t>Ichigo's Tensa Zangetsu Bankai</t>
+  </si>
+  <si>
+    <t>Ichigo's Tensa Zangetsu Bankai v2</t>
+  </si>
+  <si>
+    <t>fullbring.jpg</t>
+  </si>
+  <si>
+    <t>bankai.jpg</t>
+  </si>
+  <si>
+    <t>bankai v2.jpg</t>
   </si>
 </sst>
 </file>
@@ -532,10 +877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B157F8F3-2502-4E5D-9075-AC3F10DBE2D5}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,13 +907,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1">
         <v>8500</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -576,7 +921,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>4200</v>
@@ -585,12 +930,12 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>1200</v>
@@ -599,12 +944,12 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>2000</v>
@@ -613,12 +958,12 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>2200</v>
@@ -627,12 +972,12 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>1700</v>
@@ -641,12 +986,12 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>1700</v>
@@ -655,12 +1000,12 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1">
         <v>1700</v>
@@ -669,12 +1014,12 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>1700</v>
@@ -683,12 +1028,12 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1">
         <v>1700</v>
@@ -697,12 +1042,12 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1">
         <v>1700</v>
@@ -711,12 +1056,12 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1">
         <v>10500</v>
@@ -725,12 +1070,12 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1">
         <v>1600</v>
@@ -739,12 +1084,12 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1">
         <v>1200</v>
@@ -753,12 +1098,12 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1">
         <v>1600</v>
@@ -767,12 +1112,12 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1">
         <v>3000</v>
@@ -781,12 +1126,12 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1">
         <v>4500</v>
@@ -795,12 +1140,12 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="1">
         <v>10500</v>
@@ -809,7 +1154,805 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="1">
+        <v>6000</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" s="1">
+        <v>6000</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="1">
+        <v>1400</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="1">
+        <v>900</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="1">
+        <v>5200</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>149</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1800</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>117</v>
+      </c>
+      <c r="B61" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>154</v>
+      </c>
+      <c r="B62" s="1">
+        <v>3500</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>118</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>148</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>122</v>
+      </c>
+      <c r="B66" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>120</v>
+      </c>
+      <c r="B68" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>121</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>123</v>
+      </c>
+      <c r="B70" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1700</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>125</v>
+      </c>
+      <c r="B72" s="1">
+        <v>700</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" s="1">
+        <v>700</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>155</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C74" t="s">
+        <v>44</v>
+      </c>
+      <c r="D74" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>156</v>
+      </c>
+      <c r="B75" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C75" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C76" t="s">
+        <v>44</v>
+      </c>
+      <c r="D76" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
metal katana pre order added
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF991C73-C307-4560-B932-F0E402CF7FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E650D2B-855B-4553-A87F-6790D4C0F6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="735" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
+    <workbookView xWindow="4140" yWindow="1080" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="179">
   <si>
     <t>Product</t>
   </si>
@@ -517,6 +517,60 @@
   </si>
   <si>
     <t>bankai v2.jpg</t>
+  </si>
+  <si>
+    <t>Shusui Katana [Metal]</t>
+  </si>
+  <si>
+    <t>Wado Ichimonji Katana [Metal]</t>
+  </si>
+  <si>
+    <t>Enma Katana [Metal]</t>
+  </si>
+  <si>
+    <t>Enma Black Katana [Metal]</t>
+  </si>
+  <si>
+    <t>Ame No Habikiri Katana [Metal]</t>
+  </si>
+  <si>
+    <t>Tanjiro's Old Nichrin [Metal]</t>
+  </si>
+  <si>
+    <t>Tanjiro's New Nichrin [Metal]</t>
+  </si>
+  <si>
+    <t>Inosuke's Nichrin [Metal]</t>
+  </si>
+  <si>
+    <t>Sanemi's Nichrin [Metal]</t>
+  </si>
+  <si>
+    <t>shusui metal.jpg</t>
+  </si>
+  <si>
+    <t>wado metal.jpg</t>
+  </si>
+  <si>
+    <t>enma metal.jpg</t>
+  </si>
+  <si>
+    <t>ame metal.jpg</t>
+  </si>
+  <si>
+    <t>enma bl metal.jpg</t>
+  </si>
+  <si>
+    <t>tanjiro old metal.jpg</t>
+  </si>
+  <si>
+    <t>tanjiro new metal.jpg</t>
+  </si>
+  <si>
+    <t>ino metal.jpg</t>
+  </si>
+  <si>
+    <t>sanemi metal.jpg</t>
   </si>
 </sst>
 </file>
@@ -877,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B157F8F3-2502-4E5D-9075-AC3F10DBE2D5}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,133 +1213,133 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="B20" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>162</v>
       </c>
       <c r="B21" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>163</v>
       </c>
       <c r="B22" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C22" t="s">
         <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>164</v>
       </c>
       <c r="B23" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="B24" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C24" t="s">
         <v>44</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>166</v>
       </c>
       <c r="B25" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C25" t="s">
         <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>167</v>
       </c>
       <c r="B26" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C26" t="s">
         <v>44</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>168</v>
       </c>
       <c r="B27" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C27" t="s">
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="B28" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C28" t="s">
         <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B29" s="1">
         <v>2300</v>
@@ -1294,12 +1348,12 @@
         <v>44</v>
       </c>
       <c r="D29" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B30" s="1">
         <v>2300</v>
@@ -1308,12 +1362,12 @@
         <v>44</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1">
         <v>2300</v>
@@ -1322,12 +1376,12 @@
         <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B32" s="1">
         <v>2300</v>
@@ -1336,12 +1390,12 @@
         <v>44</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1">
         <v>2300</v>
@@ -1350,12 +1404,12 @@
         <v>44</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B34" s="1">
         <v>2300</v>
@@ -1364,12 +1418,12 @@
         <v>44</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1">
         <v>2300</v>
@@ -1378,12 +1432,12 @@
         <v>44</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B36" s="1">
         <v>2300</v>
@@ -1392,12 +1446,12 @@
         <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1">
         <v>2300</v>
@@ -1406,12 +1460,12 @@
         <v>44</v>
       </c>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="B38" s="1">
         <v>2300</v>
@@ -1420,12 +1474,12 @@
         <v>44</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B39" s="1">
         <v>2300</v>
@@ -1434,12 +1488,12 @@
         <v>44</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B40" s="1">
         <v>2300</v>
@@ -1448,12 +1502,12 @@
         <v>44</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1">
         <v>2300</v>
@@ -1462,12 +1516,12 @@
         <v>44</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1">
         <v>2300</v>
@@ -1476,482 +1530,608 @@
         <v>44</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1">
-        <v>6000</v>
+        <v>2300</v>
       </c>
       <c r="C43" t="s">
         <v>44</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="B44" s="1">
-        <v>2200</v>
+        <v>2300</v>
       </c>
       <c r="C44" t="s">
         <v>44</v>
       </c>
       <c r="D44" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="B45" s="1">
-        <v>2200</v>
+        <v>2300</v>
       </c>
       <c r="C45" t="s">
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1">
-        <v>6000</v>
+        <v>2300</v>
       </c>
       <c r="C46" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="B47" s="1">
-        <v>1400</v>
+        <v>2300</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="B48" s="1">
-        <v>900</v>
+        <v>2300</v>
       </c>
       <c r="C48" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D48" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="B49" s="1">
-        <v>2200</v>
+        <v>2300</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D49" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="B50" s="1">
-        <v>5200</v>
+        <v>2300</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D50" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>149</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>153</v>
+        <v>77</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2300</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D51" t="s">
-        <v>151</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>150</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>153</v>
+        <v>78</v>
+      </c>
+      <c r="B52" s="1">
+        <v>6000</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D52" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B53" s="1">
         <v>2200</v>
       </c>
       <c r="C53" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D53" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="B54" s="1">
-        <v>2000</v>
+        <v>2200</v>
       </c>
       <c r="C54" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B55" s="1">
-        <v>1000</v>
+        <v>6000</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B56" s="1">
-        <v>1800</v>
+        <v>1400</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B57" s="1">
-        <v>3500</v>
+        <v>900</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B58" s="1">
-        <v>3500</v>
+        <v>2200</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B59" s="1">
-        <v>3500</v>
+        <v>5200</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>116</v>
-      </c>
-      <c r="B60" s="1">
-        <v>3500</v>
+        <v>149</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" s="1">
-        <v>3500</v>
+        <v>150</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>105</v>
       </c>
       <c r="B62" s="1">
-        <v>3500</v>
+        <v>2200</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B63" s="1">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B64" s="1">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="B65" s="1">
-        <v>2500</v>
+        <v>1800</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B66" s="1">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B67" s="1">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B68" s="1">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
       </c>
       <c r="D68" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B69" s="1">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B70" s="1">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="B71" s="1">
-        <v>1700</v>
+        <v>3500</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="B72" s="1">
-        <v>700</v>
+        <v>2500</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B73" s="1">
-        <v>700</v>
+        <v>2500</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B74" s="1">
         <v>2500</v>
       </c>
       <c r="C74" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B75" s="1">
         <v>2500</v>
       </c>
       <c r="C75" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="B76" s="1">
         <v>2500</v>
       </c>
       <c r="C76" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="D76" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C78" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>124</v>
+      </c>
+      <c r="B80" s="1">
+        <v>1700</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81" s="1">
+        <v>700</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>126</v>
+      </c>
+      <c r="B82" s="1">
+        <v>700</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>155</v>
+      </c>
+      <c r="B83" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D83" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>156</v>
+      </c>
+      <c r="B84" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C84" t="s">
+        <v>44</v>
+      </c>
+      <c r="D84" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>157</v>
+      </c>
+      <c r="B85" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C85" t="s">
+        <v>44</v>
+      </c>
+      <c r="D85" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pre-order minifig set update
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E650D2B-855B-4553-A87F-6790D4C0F6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7CCCFE-08C7-45FE-8698-92A1636B59C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1080" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
+    <workbookView xWindow="4050" yWindow="2340" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="233">
   <si>
     <t>Product</t>
   </si>
@@ -571,6 +571,168 @@
   </si>
   <si>
     <t>sanemi metal.jpg</t>
+  </si>
+  <si>
+    <t>Demon Slayer Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>Naruto Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>Naruto Set v2 (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>Marvel's Spiderman Game Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>Football Stars Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>Deadpool &amp; Wolverine Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>naruto set.jpg</t>
+  </si>
+  <si>
+    <t>akatsuki set.jpg</t>
+  </si>
+  <si>
+    <t>bleach set.jpg</t>
+  </si>
+  <si>
+    <t>haikyuu set.jpg</t>
+  </si>
+  <si>
+    <t>aot set.jpg</t>
+  </si>
+  <si>
+    <t>aot set 2.jpg</t>
+  </si>
+  <si>
+    <t>jojo set.jpg</t>
+  </si>
+  <si>
+    <t>jojo set 2.jpg</t>
+  </si>
+  <si>
+    <t>kaiju set.jpg</t>
+  </si>
+  <si>
+    <t>boys set.jpg</t>
+  </si>
+  <si>
+    <t>boys set 2.jpg</t>
+  </si>
+  <si>
+    <t>loki set.jpg</t>
+  </si>
+  <si>
+    <t>loki set 2.jpg</t>
+  </si>
+  <si>
+    <t>ds set.jpg</t>
+  </si>
+  <si>
+    <t>tmnt set.jpg</t>
+  </si>
+  <si>
+    <t>football set.jpg</t>
+  </si>
+  <si>
+    <t>spiderman set.jpg</t>
+  </si>
+  <si>
+    <t>spiderman set 2.jpg</t>
+  </si>
+  <si>
+    <t>dp wol set.jpg</t>
+  </si>
+  <si>
+    <t>naruto set 2.jpg</t>
+  </si>
+  <si>
+    <t>Multiverse of Madness + The Boys Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>Punisher &amp; Daredevil Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>X-97 Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>Akatsuki Set (12 minifigure)</t>
+  </si>
+  <si>
+    <t>Attack on Titan Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Attack on Titan Set v2 (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Bleach Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Jojo's Bizzare Adventure Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Jojo's Bizzare Adventure Set v2 (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Kaiju no.08 Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>The Boys Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Haikyuu Set (9 minifigure)</t>
+  </si>
+  <si>
+    <t>The Boys Set v2 (7 minifigure)</t>
+  </si>
+  <si>
+    <t>Loki TV Series Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Loki TV Series Set v2 (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Tinage Mutant Ninja Turtles Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Spiderman-Into the Spider Verse Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>One Piece KDL Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>One Piece DY Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>One Piece TP Set (8 minifigure)</t>
+  </si>
+  <si>
+    <t>Marvel TV series Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>ran set.jpg</t>
+  </si>
+  <si>
+    <t>punisher set.jpg</t>
+  </si>
+  <si>
+    <t>xmen spiderman set.jpg</t>
+  </si>
+  <si>
+    <t>one piece dy set.jpg</t>
+  </si>
+  <si>
+    <t>one piece tp set.jpg</t>
+  </si>
+  <si>
+    <t>one piece kdl set.jpg</t>
+  </si>
+  <si>
+    <t>ran marvel set.jpg</t>
   </si>
 </sst>
 </file>
@@ -931,15 +1093,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B157F8F3-2502-4E5D-9075-AC3F10DBE2D5}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
@@ -2135,6 +2297,384 @@
         <v>160</v>
       </c>
     </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>180</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>181</v>
+      </c>
+      <c r="B87" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>208</v>
+      </c>
+      <c r="B88" s="1">
+        <v>2400</v>
+      </c>
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>209</v>
+      </c>
+      <c r="B89" s="1">
+        <v>2100</v>
+      </c>
+      <c r="C89" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>210</v>
+      </c>
+      <c r="B90" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C90" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>211</v>
+      </c>
+      <c r="B91" s="1">
+        <v>2150</v>
+      </c>
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>212</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>213</v>
+      </c>
+      <c r="B93" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C93" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>214</v>
+      </c>
+      <c r="B94" s="1">
+        <v>2050</v>
+      </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>215</v>
+      </c>
+      <c r="B95" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>217</v>
+      </c>
+      <c r="B96" s="1">
+        <v>1400</v>
+      </c>
+      <c r="C96" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>216</v>
+      </c>
+      <c r="B97" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C97" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>218</v>
+      </c>
+      <c r="B98" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>219</v>
+      </c>
+      <c r="B99" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>179</v>
+      </c>
+      <c r="B100" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C100" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>220</v>
+      </c>
+      <c r="B101" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C101" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>183</v>
+      </c>
+      <c r="B102" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C102" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>182</v>
+      </c>
+      <c r="B103" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C103" t="s">
+        <v>9</v>
+      </c>
+      <c r="D103" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>221</v>
+      </c>
+      <c r="B104" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C104" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>184</v>
+      </c>
+      <c r="B105" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C105" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>205</v>
+      </c>
+      <c r="B106" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C106" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>207</v>
+      </c>
+      <c r="B107" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C107" t="s">
+        <v>9</v>
+      </c>
+      <c r="D107" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>206</v>
+      </c>
+      <c r="B108" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C108" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>223</v>
+      </c>
+      <c r="B109" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C109" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>224</v>
+      </c>
+      <c r="B110" s="1">
+        <v>1800</v>
+      </c>
+      <c r="C110" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>222</v>
+      </c>
+      <c r="B111" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C111" t="s">
+        <v>9</v>
+      </c>
+      <c r="D111" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>225</v>
+      </c>
+      <c r="B112" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C112" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
minifigure set, pokemon figure + stock update + back to top added in pre-order
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7CCCFE-08C7-45FE-8698-92A1636B59C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2116FC3A-0A88-4953-AB31-CEFF3AD8F28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="2340" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
+    <workbookView xWindow="3075" yWindow="1110" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="293">
   <si>
     <t>Product</t>
   </si>
@@ -733,6 +733,186 @@
   </si>
   <si>
     <t>ran marvel set.jpg</t>
+  </si>
+  <si>
+    <t>Charizard Battle Scene Figure</t>
+  </si>
+  <si>
+    <t>Dragonite Battle Scene Figure</t>
+  </si>
+  <si>
+    <t>Arcanine Battle Scene Figure</t>
+  </si>
+  <si>
+    <t>Lapras Battle Scene Figure</t>
+  </si>
+  <si>
+    <t>Blastoise Battle Scene Figure</t>
+  </si>
+  <si>
+    <t>Venasaur Battle Scene Figure</t>
+  </si>
+  <si>
+    <t>charizard lang.jpg</t>
+  </si>
+  <si>
+    <t>dragonite lang.jpg</t>
+  </si>
+  <si>
+    <t>arcanine lang.jpg</t>
+  </si>
+  <si>
+    <t>lapras lang.jpg</t>
+  </si>
+  <si>
+    <t>blastoise lang.jpg</t>
+  </si>
+  <si>
+    <t>venasaur lang.jpg</t>
+  </si>
+  <si>
+    <t>Charizard + Charmander Duo Keepley Figure</t>
+  </si>
+  <si>
+    <t>Venasaur + Bulbasaur Duo Keepley Figure</t>
+  </si>
+  <si>
+    <t>Blastoise + Squirtle Duo Keepley Figure</t>
+  </si>
+  <si>
+    <t>Mewtwo + Mew Duo Keepley Figure</t>
+  </si>
+  <si>
+    <t>Greninja Keepley Figure</t>
+  </si>
+  <si>
+    <t>Metagross Keepley Figure</t>
+  </si>
+  <si>
+    <t>Lucario Keepley Figure</t>
+  </si>
+  <si>
+    <t>Pikachu Keepley Figure</t>
+  </si>
+  <si>
+    <t>Meowth Keepley Figure</t>
+  </si>
+  <si>
+    <t>Cinderace Keepley Figure</t>
+  </si>
+  <si>
+    <t>charizard keep.jpg</t>
+  </si>
+  <si>
+    <t>venasaur keep.jpg</t>
+  </si>
+  <si>
+    <t>blastoise keep.jpg</t>
+  </si>
+  <si>
+    <t>mewtwo keep.jpg</t>
+  </si>
+  <si>
+    <t>greninja keep.jpg</t>
+  </si>
+  <si>
+    <t>metagross keep.jpg</t>
+  </si>
+  <si>
+    <t>lucario keep.jpg</t>
+  </si>
+  <si>
+    <t>pikachu keep.jpg</t>
+  </si>
+  <si>
+    <t>cinderace keep.jpg</t>
+  </si>
+  <si>
+    <t>meowth keep.jpg</t>
+  </si>
+  <si>
+    <t>Multiverse Saga Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>multiverse saga set.jpg</t>
+  </si>
+  <si>
+    <t>Harry Potter Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>hp set.jpg</t>
+  </si>
+  <si>
+    <t>Chainsawman Diorama</t>
+  </si>
+  <si>
+    <t>chainsawman diorama.jpg</t>
+  </si>
+  <si>
+    <t>DC set (6 Minifigure)</t>
+  </si>
+  <si>
+    <t>One Piece Marine Set (7 Minifigure)</t>
+  </si>
+  <si>
+    <t>Fantastic 4 Set (5 Minifgure)</t>
+  </si>
+  <si>
+    <t>Demon Slayer Demon Set (10 Minifigure)</t>
+  </si>
+  <si>
+    <t>Demon Slayer Hashira Set (9 Minifigure)</t>
+  </si>
+  <si>
+    <t>One Piece Wano Set (8 Minifigure)</t>
+  </si>
+  <si>
+    <t>Ironman Mark I</t>
+  </si>
+  <si>
+    <t>Thanos Big Figure</t>
+  </si>
+  <si>
+    <t>Marvels Set (7 Minifigure)</t>
+  </si>
+  <si>
+    <t>Bleach Set (Any 8 Minifigure)</t>
+  </si>
+  <si>
+    <t>marine set.jpg</t>
+  </si>
+  <si>
+    <t>dc set.jpg</t>
+  </si>
+  <si>
+    <t>hashira set.jpg</t>
+  </si>
+  <si>
+    <t>thanos big.jpg</t>
+  </si>
+  <si>
+    <t>f4 set.jpg</t>
+  </si>
+  <si>
+    <t>ds demon set.jpg</t>
+  </si>
+  <si>
+    <t>one piece wano set.jpg</t>
+  </si>
+  <si>
+    <t>ironman mark 1.jpg</t>
+  </si>
+  <si>
+    <t>bleach set 2.jpg</t>
+  </si>
+  <si>
+    <t>marvels set.jpg</t>
+  </si>
+  <si>
+    <t>Chainsawman Set (10 Minifigure)</t>
+  </si>
+  <si>
+    <t>chainsawman set.jpg</t>
   </si>
 </sst>
 </file>
@@ -1093,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B157F8F3-2502-4E5D-9075-AC3F10DBE2D5}">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D112" sqref="D112"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,7 +1284,7 @@
     <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2673,6 +2853,426 @@
       </c>
       <c r="D112" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>233</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C113" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>234</v>
+      </c>
+      <c r="B114" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C114" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>235</v>
+      </c>
+      <c r="B115" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C115" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>236</v>
+      </c>
+      <c r="B116" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C116" t="s">
+        <v>6</v>
+      </c>
+      <c r="D116" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>237</v>
+      </c>
+      <c r="B117" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C117" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>238</v>
+      </c>
+      <c r="B118" s="1">
+        <v>2000</v>
+      </c>
+      <c r="C118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>245</v>
+      </c>
+      <c r="B119" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C119" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>246</v>
+      </c>
+      <c r="B120" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C120" t="s">
+        <v>6</v>
+      </c>
+      <c r="D120" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>247</v>
+      </c>
+      <c r="B121" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C121" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>248</v>
+      </c>
+      <c r="B122" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C122" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>249</v>
+      </c>
+      <c r="B123" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C123" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>250</v>
+      </c>
+      <c r="B124" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C124" t="s">
+        <v>6</v>
+      </c>
+      <c r="D124" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>251</v>
+      </c>
+      <c r="B125" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C125" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>252</v>
+      </c>
+      <c r="B126" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C126" t="s">
+        <v>6</v>
+      </c>
+      <c r="D126" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>254</v>
+      </c>
+      <c r="B127" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C127" t="s">
+        <v>6</v>
+      </c>
+      <c r="D127" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>253</v>
+      </c>
+      <c r="B128" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C128" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>265</v>
+      </c>
+      <c r="B129" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C129" t="s">
+        <v>9</v>
+      </c>
+      <c r="D129" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>267</v>
+      </c>
+      <c r="B130" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C130" t="s">
+        <v>9</v>
+      </c>
+      <c r="D130" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>269</v>
+      </c>
+      <c r="B131" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C131" t="s">
+        <v>4</v>
+      </c>
+      <c r="D131" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>272</v>
+      </c>
+      <c r="B132" s="1">
+        <v>1950</v>
+      </c>
+      <c r="C132" t="s">
+        <v>9</v>
+      </c>
+      <c r="D132" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>271</v>
+      </c>
+      <c r="B133" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C133" t="s">
+        <v>9</v>
+      </c>
+      <c r="D133" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>273</v>
+      </c>
+      <c r="B134" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C134" t="s">
+        <v>9</v>
+      </c>
+      <c r="D134" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>274</v>
+      </c>
+      <c r="B135" s="1">
+        <v>2500</v>
+      </c>
+      <c r="C135" t="s">
+        <v>9</v>
+      </c>
+      <c r="D135" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>275</v>
+      </c>
+      <c r="B136" s="1">
+        <v>2100</v>
+      </c>
+      <c r="C136" t="s">
+        <v>9</v>
+      </c>
+      <c r="D136" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>276</v>
+      </c>
+      <c r="B137" s="1">
+        <v>2080</v>
+      </c>
+      <c r="C137" t="s">
+        <v>9</v>
+      </c>
+      <c r="D137" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>277</v>
+      </c>
+      <c r="B138" s="1">
+        <v>450</v>
+      </c>
+      <c r="C138" t="s">
+        <v>9</v>
+      </c>
+      <c r="D138" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>279</v>
+      </c>
+      <c r="B139" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C139" t="s">
+        <v>9</v>
+      </c>
+      <c r="D139" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>280</v>
+      </c>
+      <c r="B140" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C140" t="s">
+        <v>9</v>
+      </c>
+      <c r="D140" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>278</v>
+      </c>
+      <c r="B141" s="1">
+        <v>750</v>
+      </c>
+      <c r="C141" t="s">
+        <v>9</v>
+      </c>
+      <c r="D141" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>291</v>
+      </c>
+      <c r="B142" s="1">
+        <v>2300</v>
+      </c>
+      <c r="C142" t="s">
+        <v>9</v>
+      </c>
+      <c r="D142" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stock update blockee pokemon added
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2116FC3A-0A88-4953-AB31-CEFF3AD8F28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB45B03D-B43B-4996-9587-692905C95AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="1110" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
+    <workbookView xWindow="6450" yWindow="1905" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="301">
   <si>
     <t>Product</t>
   </si>
@@ -913,6 +913,30 @@
   </si>
   <si>
     <t>chainsawman set.jpg</t>
+  </si>
+  <si>
+    <t>Charizard Blockee Figure</t>
+  </si>
+  <si>
+    <t>Greninja Blockee Figure</t>
+  </si>
+  <si>
+    <t>Meowscrada Blockee Figure</t>
+  </si>
+  <si>
+    <t>Ceruledge Blockee Figure</t>
+  </si>
+  <si>
+    <t>charizard blockee.jpg</t>
+  </si>
+  <si>
+    <t>greninja blockee.jpg</t>
+  </si>
+  <si>
+    <t>grass blockee.jpg</t>
+  </si>
+  <si>
+    <t>sword blockee.jpg</t>
   </si>
 </sst>
 </file>
@@ -1273,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B157F8F3-2502-4E5D-9075-AC3F10DBE2D5}">
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2941,119 +2965,119 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>245</v>
+        <v>293</v>
       </c>
       <c r="B119" s="1">
-        <v>2200</v>
+        <v>3750</v>
       </c>
       <c r="C119" t="s">
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>255</v>
+        <v>297</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>246</v>
+        <v>294</v>
       </c>
       <c r="B120" s="1">
-        <v>2200</v>
+        <v>3200</v>
       </c>
       <c r="C120" t="s">
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>256</v>
+        <v>298</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>247</v>
+        <v>295</v>
       </c>
       <c r="B121" s="1">
-        <v>2200</v>
+        <v>3200</v>
       </c>
       <c r="C121" t="s">
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>257</v>
+        <v>299</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>248</v>
+        <v>296</v>
       </c>
       <c r="B122" s="1">
-        <v>2200</v>
+        <v>3350</v>
       </c>
       <c r="C122" t="s">
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>258</v>
+        <v>300</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B123" s="1">
-        <v>1200</v>
+        <v>2200</v>
       </c>
       <c r="C123" t="s">
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B124" s="1">
-        <v>1200</v>
+        <v>2200</v>
       </c>
       <c r="C124" t="s">
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B125" s="1">
-        <v>1200</v>
+        <v>2200</v>
       </c>
       <c r="C125" t="s">
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B126" s="1">
-        <v>1200</v>
+        <v>2200</v>
       </c>
       <c r="C126" t="s">
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B127" s="1">
         <v>1200</v>
@@ -3062,12 +3086,12 @@
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B128" s="1">
         <v>1200</v>
@@ -3076,202 +3100,258 @@
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="B129" s="1">
-        <v>1600</v>
+        <v>1200</v>
       </c>
       <c r="C129" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="B130" s="1">
-        <v>1600</v>
+        <v>1200</v>
       </c>
       <c r="C130" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
       <c r="B131" s="1">
-        <v>1600</v>
+        <v>1200</v>
       </c>
       <c r="C131" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>272</v>
+        <v>253</v>
       </c>
       <c r="B132" s="1">
-        <v>1950</v>
+        <v>1200</v>
       </c>
       <c r="C132" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B133" s="1">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="C133" t="s">
         <v>9</v>
       </c>
       <c r="D133" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B134" s="1">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="C134" t="s">
         <v>9</v>
       </c>
       <c r="D134" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B135" s="1">
-        <v>2500</v>
+        <v>1600</v>
       </c>
       <c r="C135" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D135" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B136" s="1">
-        <v>2100</v>
+        <v>1950</v>
       </c>
       <c r="C136" t="s">
         <v>9</v>
       </c>
       <c r="D136" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B137" s="1">
-        <v>2080</v>
+        <v>1000</v>
       </c>
       <c r="C137" t="s">
         <v>9</v>
       </c>
       <c r="D137" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B138" s="1">
-        <v>450</v>
+        <v>1000</v>
       </c>
       <c r="C138" t="s">
         <v>9</v>
       </c>
       <c r="D138" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B139" s="1">
-        <v>1200</v>
+        <v>2500</v>
       </c>
       <c r="C139" t="s">
         <v>9</v>
       </c>
       <c r="D139" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B140" s="1">
-        <v>1600</v>
+        <v>2100</v>
       </c>
       <c r="C140" t="s">
         <v>9</v>
       </c>
       <c r="D140" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B141" s="1">
-        <v>750</v>
+        <v>2080</v>
       </c>
       <c r="C141" t="s">
         <v>9</v>
       </c>
       <c r="D141" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>277</v>
+      </c>
+      <c r="B142" s="1">
+        <v>450</v>
+      </c>
+      <c r="C142" t="s">
+        <v>9</v>
+      </c>
+      <c r="D142" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>279</v>
+      </c>
+      <c r="B143" s="1">
+        <v>1200</v>
+      </c>
+      <c r="C143" t="s">
+        <v>9</v>
+      </c>
+      <c r="D143" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>280</v>
+      </c>
+      <c r="B144" s="1">
+        <v>1600</v>
+      </c>
+      <c r="C144" t="s">
+        <v>9</v>
+      </c>
+      <c r="D144" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>278</v>
+      </c>
+      <c r="B145" s="1">
+        <v>750</v>
+      </c>
+      <c r="C145" t="s">
+        <v>9</v>
+      </c>
+      <c r="D145" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>291</v>
       </c>
-      <c r="B142" s="1">
+      <c r="B146" s="1">
         <v>2300</v>
       </c>
-      <c r="C142" t="s">
-        <v>9</v>
-      </c>
-      <c r="D142" t="s">
+      <c r="C146" t="s">
+        <v>9</v>
+      </c>
+      <c r="D146" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
gunpla added price update
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE000652-C628-4B14-8B40-579DE28C2216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB40A0A-FE9C-4E9D-9A2B-7B909230CE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="2595" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="325">
   <si>
     <t>Product</t>
   </si>
@@ -963,34 +963,52 @@
     <t>display stand gundam.jpg</t>
   </si>
   <si>
-    <t>[HG] Glacier Transient Bootleg [1:144]</t>
-  </si>
-  <si>
-    <t>[HG] Transient Bootleg [1:144]</t>
-  </si>
-  <si>
-    <t>[RG] RX-78 BANDAI [1:144]</t>
-  </si>
-  <si>
     <t>[HG] Freedom Gundam Bootleg [1:144]</t>
   </si>
   <si>
-    <t>[HG] RX-178 Bootleg [1:144]</t>
-  </si>
-  <si>
-    <t>[FM] Gundam Aerial Bootleg [1:100]</t>
-  </si>
-  <si>
-    <t>[HG] Load Astray with Cloack Bootleg [1:144]</t>
-  </si>
-  <si>
-    <t>[HG] Gundam Aerial Bootleg [1:144]</t>
-  </si>
-  <si>
-    <t>[MG] Freedom 2.0  DABAN[1:100]</t>
-  </si>
-  <si>
     <t>mg freedom 2.jpg</t>
+  </si>
+  <si>
+    <t>green zaku.jpg</t>
+  </si>
+  <si>
+    <t>red zaku.jpg</t>
+  </si>
+  <si>
+    <t>mg rx78.jpg</t>
+  </si>
+  <si>
+    <t>[MG] RX-78 Ver.Ka [BANDAI] [1:100]</t>
+  </si>
+  <si>
+    <t>[RG] RX-78 [BANDAI] [1:144]</t>
+  </si>
+  <si>
+    <t>[MG] Freedom 2.0  [DABAN] [1:100]</t>
+  </si>
+  <si>
+    <t>[HG] Gundam Aerial (Bootleg) [1:144]</t>
+  </si>
+  <si>
+    <t>[HG] Load Astray with Cloak (Bootleg) [1:144]</t>
+  </si>
+  <si>
+    <t>[FM] Gundam Aerial (Bootleg) [1:100]</t>
+  </si>
+  <si>
+    <t>[HG] MS-06 Zaku II (Bootleg) [1:144]</t>
+  </si>
+  <si>
+    <t>[HG] Zaku II [Psyco Zaku] (Bootleg) [1:144]</t>
+  </si>
+  <si>
+    <t>[HG] RX-178 [JMS] [1:144]</t>
+  </si>
+  <si>
+    <t>[HG] Transient [JMS] [1:144]</t>
+  </si>
+  <si>
+    <t>[HG] Glacier Transient [JMS] [1:144]</t>
   </si>
 </sst>
 </file>
@@ -1351,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B157F8F3-2502-4E5D-9075-AC3F10DBE2D5}">
-  <dimension ref="A1:D155"/>
+  <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A157" sqref="A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1455,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="B6" s="1">
         <v>5600</v>
@@ -1451,49 +1469,49 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B7" s="1">
-        <v>5600</v>
+        <v>12000</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="B8" s="1">
-        <v>2200</v>
+        <v>5500</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>309</v>
       </c>
       <c r="B9" s="1">
-        <v>1700</v>
+        <v>1500</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
         <v>1700</v>
@@ -1502,12 +1520,12 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>1700</v>
@@ -1516,12 +1534,12 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
         <v>1700</v>
@@ -1530,12 +1548,12 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1">
         <v>1700</v>
@@ -1544,12 +1562,12 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>1700</v>
@@ -1558,124 +1576,124 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1">
-        <v>10500</v>
+        <v>1700</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1">
-        <v>1600</v>
+        <v>10500</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1">
-        <v>1200</v>
+        <v>1600</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1">
-        <v>1600</v>
+        <v>1200</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1">
-        <v>3000</v>
+        <v>1600</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1">
-        <v>4500</v>
+        <v>3000</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1">
-        <v>10500</v>
+        <v>4500</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1">
-        <v>5700</v>
+        <v>10500</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B23" s="1">
         <v>5700</v>
@@ -1684,12 +1702,12 @@
         <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B24" s="1">
         <v>5700</v>
@@ -1698,12 +1716,12 @@
         <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B25" s="1">
         <v>5700</v>
@@ -1712,12 +1730,12 @@
         <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="1">
         <v>5700</v>
@@ -1726,12 +1744,12 @@
         <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27" s="1">
         <v>5700</v>
@@ -1740,12 +1758,12 @@
         <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B28" s="1">
         <v>5700</v>
@@ -1754,12 +1772,12 @@
         <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" s="1">
         <v>5700</v>
@@ -1768,12 +1786,12 @@
         <v>43</v>
       </c>
       <c r="D29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B30" s="1">
         <v>5700</v>
@@ -1782,26 +1800,26 @@
         <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="B31" s="1">
-        <v>2300</v>
+        <v>5700</v>
       </c>
       <c r="C31" t="s">
         <v>43</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1">
         <v>2300</v>
@@ -1810,12 +1828,12 @@
         <v>43</v>
       </c>
       <c r="D32" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B33" s="1">
         <v>2300</v>
@@ -1824,12 +1842,12 @@
         <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="1">
         <v>2300</v>
@@ -1838,12 +1856,12 @@
         <v>43</v>
       </c>
       <c r="D34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" s="1">
         <v>2300</v>
@@ -1852,12 +1870,12 @@
         <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="1">
         <v>2300</v>
@@ -1866,12 +1884,12 @@
         <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B37" s="1">
         <v>2300</v>
@@ -1880,12 +1898,12 @@
         <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="1">
         <v>2300</v>
@@ -1894,12 +1912,12 @@
         <v>43</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" s="1">
         <v>2300</v>
@@ -1908,12 +1926,12 @@
         <v>43</v>
       </c>
       <c r="D39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B40" s="1">
         <v>2300</v>
@@ -1922,12 +1940,12 @@
         <v>43</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B41" s="1">
         <v>2300</v>
@@ -1936,12 +1954,12 @@
         <v>43</v>
       </c>
       <c r="D41" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B42" s="1">
         <v>2300</v>
@@ -1950,12 +1968,12 @@
         <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B43" s="1">
         <v>2300</v>
@@ -1964,12 +1982,12 @@
         <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B44" s="1">
         <v>2300</v>
@@ -1978,12 +1996,12 @@
         <v>43</v>
       </c>
       <c r="D44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" s="1">
         <v>2300</v>
@@ -1992,12 +2010,12 @@
         <v>43</v>
       </c>
       <c r="D45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46" s="1">
         <v>2300</v>
@@ -2006,12 +2024,12 @@
         <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B47" s="1">
         <v>2300</v>
@@ -2020,12 +2038,12 @@
         <v>43</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" s="1">
         <v>2300</v>
@@ -2034,12 +2052,12 @@
         <v>43</v>
       </c>
       <c r="D48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B49" s="1">
         <v>2300</v>
@@ -2048,12 +2066,12 @@
         <v>43</v>
       </c>
       <c r="D49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B50" s="1">
         <v>2300</v>
@@ -2062,12 +2080,12 @@
         <v>43</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B51" s="1">
         <v>2300</v>
@@ -2076,12 +2094,12 @@
         <v>43</v>
       </c>
       <c r="D51" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B52" s="1">
         <v>2300</v>
@@ -2090,12 +2108,12 @@
         <v>43</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" s="1">
         <v>2300</v>
@@ -2104,40 +2122,40 @@
         <v>43</v>
       </c>
       <c r="D53" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B54" s="1">
-        <v>6000</v>
+        <v>2300</v>
       </c>
       <c r="C54" t="s">
         <v>43</v>
       </c>
       <c r="D54" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B55" s="1">
-        <v>2200</v>
+        <v>6000</v>
       </c>
       <c r="C55" t="s">
         <v>43</v>
       </c>
       <c r="D55" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B56" s="1">
         <v>2200</v>
@@ -2146,96 +2164,96 @@
         <v>43</v>
       </c>
       <c r="D56" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B57" s="1">
-        <v>6000</v>
+        <v>2200</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="D57" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B58" s="1">
-        <v>1400</v>
+        <v>6000</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59" s="1">
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B60" s="1">
-        <v>2200</v>
+        <v>900</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" s="1">
-        <v>5200</v>
+        <v>2200</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>148</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>152</v>
+        <v>102</v>
+      </c>
+      <c r="B62" s="1">
+        <v>5200</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>152</v>
@@ -2244,82 +2262,82 @@
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>104</v>
-      </c>
-      <c r="B64" s="1">
-        <v>2200</v>
+        <v>149</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B65" s="1">
-        <v>2000</v>
+        <v>2200</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B66" s="1">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B67" s="1">
-        <v>1800</v>
+        <v>1000</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B68" s="1">
-        <v>3500</v>
+        <v>1800</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
       </c>
       <c r="D68" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B69" s="1">
         <v>3500</v>
@@ -2328,12 +2346,12 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B70" s="1">
         <v>3500</v>
@@ -2342,12 +2360,12 @@
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B71" s="1">
         <v>3500</v>
@@ -2356,12 +2374,12 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B72" s="1">
         <v>3500</v>
@@ -2370,12 +2388,12 @@
         <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="B73" s="1">
         <v>3500</v>
@@ -2384,26 +2402,26 @@
         <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="B74" s="1">
-        <v>2500</v>
+        <v>3500</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B75" s="1">
         <v>2500</v>
@@ -2412,12 +2430,12 @@
         <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
       <c r="B76" s="1">
         <v>2500</v>
@@ -2426,12 +2444,12 @@
         <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>147</v>
       </c>
       <c r="B77" s="1">
         <v>2500</v>
@@ -2440,12 +2458,12 @@
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B78" s="1">
         <v>2500</v>
@@ -2454,12 +2472,12 @@
         <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B79" s="1">
         <v>2500</v>
@@ -2468,12 +2486,12 @@
         <v>5</v>
       </c>
       <c r="D79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B80" s="1">
         <v>2500</v>
@@ -2482,12 +2500,12 @@
         <v>5</v>
       </c>
       <c r="D80" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B81" s="1">
         <v>2500</v>
@@ -2496,40 +2514,40 @@
         <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B82" s="1">
-        <v>1700</v>
+        <v>2500</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B83" s="1">
-        <v>700</v>
+        <v>1700</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
       </c>
       <c r="D83" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B84" s="1">
         <v>700</v>
@@ -2538,26 +2556,26 @@
         <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="B85" s="1">
-        <v>2500</v>
+        <v>700</v>
       </c>
       <c r="C85" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B86" s="1">
         <v>2500</v>
@@ -2566,12 +2584,12 @@
         <v>43</v>
       </c>
       <c r="D86" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B87" s="1">
         <v>2500</v>
@@ -2580,26 +2598,26 @@
         <v>43</v>
       </c>
       <c r="D87" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="B88" s="1">
-        <v>1600</v>
+        <v>2500</v>
       </c>
       <c r="C88" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="D88" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B89" s="1">
         <v>1600</v>
@@ -2608,82 +2626,82 @@
         <v>9</v>
       </c>
       <c r="D89" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="B90" s="1">
-        <v>2400</v>
+        <v>1600</v>
       </c>
       <c r="C90" t="s">
         <v>9</v>
       </c>
       <c r="D90" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B91" s="1">
-        <v>2100</v>
+        <v>2400</v>
       </c>
       <c r="C91" t="s">
         <v>9</v>
       </c>
       <c r="D91" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B92" s="1">
-        <v>2200</v>
+        <v>2100</v>
       </c>
       <c r="C92" t="s">
         <v>9</v>
       </c>
       <c r="D92" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B93" s="1">
-        <v>2150</v>
+        <v>2200</v>
       </c>
       <c r="C93" t="s">
         <v>9</v>
       </c>
       <c r="D93" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B94" s="1">
-        <v>2000</v>
+        <v>2150</v>
       </c>
       <c r="C94" t="s">
         <v>9</v>
       </c>
       <c r="D94" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B95" s="1">
         <v>2000</v>
@@ -2692,68 +2710,68 @@
         <v>9</v>
       </c>
       <c r="D95" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B96" s="1">
-        <v>2050</v>
+        <v>2000</v>
       </c>
       <c r="C96" t="s">
         <v>9</v>
       </c>
       <c r="D96" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B97" s="1">
-        <v>1600</v>
+        <v>2050</v>
       </c>
       <c r="C97" t="s">
         <v>9</v>
       </c>
       <c r="D97" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B98" s="1">
-        <v>1400</v>
+        <v>1600</v>
       </c>
       <c r="C98" t="s">
         <v>9</v>
       </c>
       <c r="D98" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B99" s="1">
-        <v>1600</v>
+        <v>1400</v>
       </c>
       <c r="C99" t="s">
         <v>9</v>
       </c>
       <c r="D99" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B100" s="1">
         <v>1600</v>
@@ -2762,12 +2780,12 @@
         <v>9</v>
       </c>
       <c r="D100" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B101" s="1">
         <v>1600</v>
@@ -2776,40 +2794,40 @@
         <v>9</v>
       </c>
       <c r="D101" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>178</v>
+        <v>218</v>
       </c>
       <c r="B102" s="1">
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="C102" t="s">
         <v>9</v>
       </c>
       <c r="D102" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>219</v>
+        <v>178</v>
       </c>
       <c r="B103" s="1">
-        <v>1600</v>
+        <v>2000</v>
       </c>
       <c r="C103" t="s">
         <v>9</v>
       </c>
       <c r="D103" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>182</v>
+        <v>219</v>
       </c>
       <c r="B104" s="1">
         <v>1600</v>
@@ -2818,12 +2836,12 @@
         <v>9</v>
       </c>
       <c r="D104" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B105" s="1">
         <v>1600</v>
@@ -2832,12 +2850,12 @@
         <v>9</v>
       </c>
       <c r="D105" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="B106" s="1">
         <v>1600</v>
@@ -2846,12 +2864,12 @@
         <v>9</v>
       </c>
       <c r="D106" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>183</v>
+        <v>220</v>
       </c>
       <c r="B107" s="1">
         <v>1600</v>
@@ -2860,12 +2878,12 @@
         <v>9</v>
       </c>
       <c r="D107" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="B108" s="1">
         <v>1600</v>
@@ -2874,12 +2892,12 @@
         <v>9</v>
       </c>
       <c r="D108" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B109" s="1">
         <v>1600</v>
@@ -2888,12 +2906,12 @@
         <v>9</v>
       </c>
       <c r="D109" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B110" s="1">
         <v>1600</v>
@@ -2902,54 +2920,54 @@
         <v>9</v>
       </c>
       <c r="D110" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="B111" s="1">
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="C111" t="s">
         <v>9</v>
       </c>
       <c r="D111" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B112" s="1">
-        <v>1800</v>
+        <v>2000</v>
       </c>
       <c r="C112" t="s">
         <v>9</v>
       </c>
       <c r="D112" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B113" s="1">
-        <v>1600</v>
+        <v>1800</v>
       </c>
       <c r="C113" t="s">
         <v>9</v>
       </c>
       <c r="D113" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B114" s="1">
         <v>1600</v>
@@ -2958,26 +2976,26 @@
         <v>9</v>
       </c>
       <c r="D114" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B115" s="1">
-        <v>2000</v>
+        <v>1600</v>
       </c>
       <c r="C115" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D115" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B116" s="1">
         <v>2000</v>
@@ -2986,12 +3004,12 @@
         <v>6</v>
       </c>
       <c r="D116" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B117" s="1">
         <v>2000</v>
@@ -3000,12 +3018,12 @@
         <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B118" s="1">
         <v>2000</v>
@@ -3014,12 +3032,12 @@
         <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B119" s="1">
         <v>2000</v>
@@ -3028,12 +3046,12 @@
         <v>6</v>
       </c>
       <c r="D119" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B120" s="1">
         <v>2000</v>
@@ -3042,40 +3060,40 @@
         <v>6</v>
       </c>
       <c r="D120" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>292</v>
+        <v>237</v>
       </c>
       <c r="B121" s="1">
-        <v>3750</v>
+        <v>2000</v>
       </c>
       <c r="C121" t="s">
         <v>6</v>
       </c>
       <c r="D121" t="s">
-        <v>296</v>
+        <v>243</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B122" s="1">
-        <v>3200</v>
+        <v>3750</v>
       </c>
       <c r="C122" t="s">
         <v>6</v>
       </c>
       <c r="D122" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B123" s="1">
         <v>3200</v>
@@ -3084,40 +3102,40 @@
         <v>6</v>
       </c>
       <c r="D123" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B124" s="1">
-        <v>3350</v>
+        <v>3200</v>
       </c>
       <c r="C124" t="s">
         <v>6</v>
       </c>
       <c r="D124" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>244</v>
+        <v>295</v>
       </c>
       <c r="B125" s="1">
-        <v>2200</v>
+        <v>3350</v>
       </c>
       <c r="C125" t="s">
         <v>6</v>
       </c>
       <c r="D125" t="s">
-        <v>254</v>
+        <v>299</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B126" s="1">
         <v>2200</v>
@@ -3126,12 +3144,12 @@
         <v>6</v>
       </c>
       <c r="D126" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B127" s="1">
         <v>2200</v>
@@ -3140,12 +3158,12 @@
         <v>6</v>
       </c>
       <c r="D127" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B128" s="1">
         <v>2200</v>
@@ -3154,26 +3172,26 @@
         <v>6</v>
       </c>
       <c r="D128" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B129" s="1">
-        <v>1200</v>
+        <v>2200</v>
       </c>
       <c r="C129" t="s">
         <v>6</v>
       </c>
       <c r="D129" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B130" s="1">
         <v>1200</v>
@@ -3182,12 +3200,12 @@
         <v>6</v>
       </c>
       <c r="D130" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B131" s="1">
         <v>1200</v>
@@ -3196,12 +3214,12 @@
         <v>6</v>
       </c>
       <c r="D131" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B132" s="1">
         <v>1200</v>
@@ -3210,12 +3228,12 @@
         <v>6</v>
       </c>
       <c r="D132" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B133" s="1">
         <v>1200</v>
@@ -3224,12 +3242,12 @@
         <v>6</v>
       </c>
       <c r="D133" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B134" s="1">
         <v>1200</v>
@@ -3238,26 +3256,26 @@
         <v>6</v>
       </c>
       <c r="D134" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="B135" s="1">
-        <v>1600</v>
+        <v>1200</v>
       </c>
       <c r="C135" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B136" s="1">
         <v>1600</v>
@@ -3266,54 +3284,54 @@
         <v>9</v>
       </c>
       <c r="D136" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B137" s="1">
         <v>1600</v>
       </c>
       <c r="C137" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D137" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B138" s="1">
-        <v>1950</v>
+        <v>1600</v>
       </c>
       <c r="C138" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D138" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B139" s="1">
-        <v>1000</v>
+        <v>1950</v>
       </c>
       <c r="C139" t="s">
         <v>9</v>
       </c>
       <c r="D139" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B140" s="1">
         <v>1000</v>
@@ -3322,216 +3340,258 @@
         <v>9</v>
       </c>
       <c r="D140" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B141" s="1">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="C141" t="s">
         <v>9</v>
       </c>
       <c r="D141" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B142" s="1">
-        <v>2100</v>
+        <v>2500</v>
       </c>
       <c r="C142" t="s">
         <v>9</v>
       </c>
       <c r="D142" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B143" s="1">
-        <v>2080</v>
+        <v>2100</v>
       </c>
       <c r="C143" t="s">
         <v>9</v>
       </c>
       <c r="D143" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B144" s="1">
-        <v>450</v>
+        <v>2080</v>
       </c>
       <c r="C144" t="s">
         <v>9</v>
       </c>
       <c r="D144" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B145" s="1">
-        <v>1200</v>
+        <v>450</v>
       </c>
       <c r="C145" t="s">
         <v>9</v>
       </c>
       <c r="D145" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B146" s="1">
-        <v>1600</v>
+        <v>1200</v>
       </c>
       <c r="C146" t="s">
         <v>9</v>
       </c>
       <c r="D146" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B147" s="1">
-        <v>750</v>
+        <v>1600</v>
       </c>
       <c r="C147" t="s">
         <v>9</v>
       </c>
       <c r="D147" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="B148" s="1">
-        <v>2300</v>
+        <v>750</v>
       </c>
       <c r="C148" t="s">
         <v>9</v>
       </c>
       <c r="D148" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>316</v>
+        <v>290</v>
       </c>
       <c r="B149" s="1">
-        <v>1500</v>
+        <v>2300</v>
       </c>
       <c r="C149" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D149" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B150" s="1">
-        <v>1600</v>
+        <v>1700</v>
       </c>
       <c r="C150" t="s">
         <v>7</v>
       </c>
       <c r="D150" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="B151" s="1">
-        <v>3500</v>
+        <v>1900</v>
       </c>
       <c r="C151" t="s">
         <v>7</v>
       </c>
       <c r="D151" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="B152" s="1">
-        <v>1500</v>
+        <v>5000</v>
       </c>
       <c r="C152" t="s">
         <v>7</v>
       </c>
       <c r="D152" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="B153" s="1">
-        <v>1500</v>
+        <v>1900</v>
       </c>
       <c r="C153" t="s">
         <v>7</v>
       </c>
       <c r="D153" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="B154" s="1">
-        <v>1500</v>
+        <v>2400</v>
       </c>
       <c r="C154" t="s">
         <v>7</v>
       </c>
       <c r="D154" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
       <c r="B155" s="1">
-        <v>850</v>
+        <v>1900</v>
       </c>
       <c r="C155" t="s">
         <v>7</v>
       </c>
       <c r="D155" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>323</v>
+      </c>
+      <c r="B156" s="1">
+        <v>1900</v>
+      </c>
+      <c r="C156" t="s">
+        <v>7</v>
+      </c>
+      <c r="D156" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>324</v>
+      </c>
+      <c r="B157" s="1">
+        <v>2200</v>
+      </c>
+      <c r="C157" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>301</v>
+      </c>
+      <c r="B158" s="1">
+        <v>850</v>
+      </c>
+      <c r="C158" t="s">
+        <v>7</v>
+      </c>
+      <c r="D158" t="s">
         <v>308</v>
       </c>
     </row>

</xml_diff>

<commit_message>
stock update 28 aug
</commit_message>
<xml_diff>
--- a/data/pre_order.xlsx
+++ b/data/pre_order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\blocks\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1D6AC3-0898-4D2B-810C-F0D8C959502A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D3C924-C092-4814-9696-D6B94DB22636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4155" yWindow="1785" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
+    <workbookView xWindow="4485" yWindow="2160" windowWidth="21600" windowHeight="11250" xr2:uid="{550C7EE9-DA08-4F00-8AFD-96A3752E125D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1377,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B157F8F3-2502-4E5D-9075-AC3F10DBE2D5}">
   <dimension ref="A1:D159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="D159" sqref="D159"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2220,7 +2220,7 @@
         <v>98</v>
       </c>
       <c r="B60" s="1">
-        <v>900</v>
+        <v>1000</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>

</xml_diff>